<commit_message>
coded item 5, fixed error item 2 coding
</commit_message>
<xml_diff>
--- a/data/error_coding/responses_to_code.xlsx
+++ b/data/error_coding/responses_to_code.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Item 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="389">
   <si>
     <t xml:space="preserve">Response</t>
   </si>
@@ -136,12 +136,12 @@
     <t xml:space="preserve">700000770</t>
   </si>
   <si>
+    <t xml:space="preserve">could be partial, so then considered concept, but forgetting one element in the top row</t>
+  </si>
+  <si>
     <t xml:space="preserve">700770700</t>
   </si>
   <si>
-    <t xml:space="preserve">could be partial, so then considered concept, but forgetting one element in the top row</t>
-  </si>
-  <si>
     <t xml:space="preserve">555555555</t>
   </si>
   <si>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">505505000</t>
   </si>
   <si>
-    <t xml:space="preserve">duplicate</t>
+    <t xml:space="preserve">duplicate_C</t>
   </si>
   <si>
     <t xml:space="preserve">partial duplicate C, changed to next color 4 to 5</t>
@@ -253,6 +253,9 @@
     <t xml:space="preserve">000500500</t>
   </si>
   <si>
+    <t xml:space="preserve">duplicate_B</t>
+  </si>
+  <si>
     <t xml:space="preserve">partial duplicate B, changed to next color 4 to 5</t>
   </si>
   <si>
@@ -313,15 +316,30 @@
     <t xml:space="preserve">660600600</t>
   </si>
   <si>
+    <t xml:space="preserve">partially correct, wrong color, but why wrong color?</t>
+  </si>
+  <si>
     <t xml:space="preserve">000000100</t>
   </si>
   <si>
     <t xml:space="preserve">700770770</t>
   </si>
   <si>
+    <t xml:space="preserve">A or C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partial matrix of A and C, one pixel off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or duplicate A or B, but one pixel off</t>
+  </si>
+  <si>
     <t xml:space="preserve">000777700</t>
   </si>
   <si>
+    <t xml:space="preserve">correct?! Or concept</t>
+  </si>
+  <si>
     <t xml:space="preserve">007007077</t>
   </si>
   <si>
@@ -346,6 +364,15 @@
     <t xml:space="preserve">777700700</t>
   </si>
   <si>
+    <t xml:space="preserve">or matrix (move middle col pixel to top, extend top row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B or C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove a pixel from the mid row</t>
+  </si>
+  <si>
     <t xml:space="preserve">070070070</t>
   </si>
   <si>
@@ -353,6 +380,9 @@
   </si>
   <si>
     <t xml:space="preserve">770770700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not sure, could be matrix</t>
   </si>
   <si>
     <t xml:space="preserve">030030077</t>
@@ -1293,11 +1323,11 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,7 +1457,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1448,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1456,7 +1486,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1464,7 +1494,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1472,7 +1502,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,7 +1510,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1488,7 +1518,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,7 +1526,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,7 +1534,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1512,7 +1542,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,7 +1550,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,7 +1558,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,7 +1566,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1544,7 +1574,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,7 +1582,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1560,7 +1590,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1568,7 +1598,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,7 +1606,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,7 +1614,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,7 +1622,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,7 +1630,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,7 +1638,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,7 +1646,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,7 +1654,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,7 +1662,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,7 +1670,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1648,7 +1678,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,7 +1686,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,7 +1694,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,7 +1702,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,7 +1710,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,7 +1718,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,7 +1726,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1704,7 +1734,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1712,7 +1742,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1750,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -1745,7 +1775,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1766,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,7 +1804,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,7 +1812,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +1820,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1798,7 +1828,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,7 +1836,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,7 +1844,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,7 +1852,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,7 +1860,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,7 +1868,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1876,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1884,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1892,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,7 +1900,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1908,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,7 +1916,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1924,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,7 +1932,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,7 +1940,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1918,7 +1948,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1956,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,7 +1964,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,7 +1972,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,7 +1980,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,7 +1988,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,7 +1996,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,7 +2004,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,7 +2012,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2007,7 +2037,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2028,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2036,7 +2066,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2044,7 +2074,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,7 +2082,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2060,7 +2090,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2068,7 +2098,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2076,7 +2106,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2084,7 +2114,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,7 +2122,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,7 +2130,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,7 +2138,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,7 +2146,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,7 +2154,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2132,7 +2162,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,7 +2170,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2148,7 +2178,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2156,7 +2186,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2164,7 +2194,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2172,7 +2202,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,7 +2210,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,7 +2218,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2226,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,7 +2234,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,7 +2242,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,7 +2250,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2228,7 +2258,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2236,7 +2266,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2244,7 +2274,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2252,7 +2282,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2260,7 +2290,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,7 +2298,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,7 +2306,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -2301,7 +2331,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2322,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,7 +2360,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,7 +2368,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,7 +2376,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2354,7 +2384,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,7 +2392,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2370,7 +2400,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,7 +2408,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,7 +2416,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,7 +2424,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2402,7 +2432,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,7 +2440,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,7 +2448,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,7 +2456,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,7 +2464,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2442,7 +2472,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2450,7 +2480,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2458,7 +2488,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,7 +2496,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -2491,7 +2521,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2512,7 +2542,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,7 +2550,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,7 +2558,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2536,7 +2566,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2544,7 +2574,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2552,7 +2582,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,7 +2590,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2568,7 +2598,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,7 +2606,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2584,7 +2614,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,7 +2622,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2600,7 +2630,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2608,7 +2638,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2646,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2624,7 +2654,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -2649,7 +2679,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2670,7 +2700,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2678,7 +2708,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2686,7 +2716,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2694,7 +2724,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2702,7 +2732,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2710,7 +2740,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2718,7 +2748,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2726,7 +2756,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2734,7 +2764,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2772,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2750,7 +2780,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2758,7 +2788,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2766,7 +2796,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,7 +2804,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2782,7 +2812,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2790,7 +2820,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,7 +2828,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2806,7 +2836,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2814,7 +2844,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2822,7 +2852,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2860,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2855,7 +2885,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.45"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2876,7 +2911,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2884,7 +2919,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2892,7 +2927,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2900,7 +2935,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,7 +2943,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2916,7 +2951,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,7 +2959,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2932,7 +2967,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2940,7 +2975,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,7 +2983,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,7 +2991,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2964,7 +2999,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2972,7 +3007,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2980,7 +3015,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2988,7 +3023,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2996,7 +3031,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3004,7 +3039,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3012,7 +3047,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3020,7 +3055,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,7 +3063,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3036,7 +3071,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -3055,16 +3090,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3241,7 +3276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
@@ -3249,7 +3284,10 @@
         <v>32</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3257,15 +3295,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3288,7 +3324,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.17"/>
@@ -3520,10 +3556,10 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.31"/>
@@ -3648,10 +3684,10 @@
         <v>71</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3659,13 +3695,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3673,7 +3709,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>5</v>
@@ -3684,13 +3720,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3698,7 +3734,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>5</v>
@@ -3709,13 +3745,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3723,13 +3759,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3737,7 +3773,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>5</v>
@@ -3748,7 +3784,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>5</v>
@@ -3759,13 +3795,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,13 +3809,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3787,13 +3823,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3814,14 +3850,15 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,7 +3880,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3853,13 +3896,19 @@
       <c r="B3" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3867,71 +3916,122 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>95</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3941,13 +4041,19 @@
       <c r="B14" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="C14" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3955,15 +4061,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>106</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3971,7 +4086,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3981,6 +4102,12 @@
       <c r="B19" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="C19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -3989,13 +4116,22 @@
       <c r="B20" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="C20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>103</v>
+        <v>112</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,7 +4139,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>104</v>
+        <v>113</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4011,7 +4150,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>105</v>
+        <v>114</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -4033,10 +4178,15 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.88"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4057,7 +4207,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4065,7 +4215,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4073,7 +4223,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4089,7 +4239,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4097,7 +4247,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4105,7 +4255,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,7 +4263,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4121,7 +4271,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4129,7 +4279,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4137,7 +4287,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4145,7 +4295,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4153,7 +4303,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4169,7 +4319,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4177,7 +4327,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4185,7 +4335,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4193,7 +4343,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4201,7 +4351,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,7 +4359,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4217,7 +4367,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4225,7 +4375,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4233,7 +4383,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4241,7 +4391,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4249,7 +4399,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4257,7 +4407,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4265,7 +4415,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4273,7 +4423,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4281,7 +4431,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4289,7 +4439,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4297,7 +4447,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4305,7 +4455,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4313,7 +4463,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4321,7 +4471,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -4346,7 +4496,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4367,7 +4517,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4375,7 +4525,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4391,7 +4541,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4399,7 +4549,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4407,7 +4557,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4415,7 +4565,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4423,7 +4573,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4431,7 +4581,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4439,7 +4589,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4447,7 +4597,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4463,7 +4613,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4471,7 +4621,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4479,7 +4629,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4487,7 +4637,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4503,7 +4653,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4511,7 +4661,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4519,7 +4669,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4527,7 +4677,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4535,7 +4685,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4543,7 +4693,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4551,7 +4701,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4559,7 +4709,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4567,7 +4717,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4575,7 +4725,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4583,7 +4733,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4591,7 +4741,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4599,7 +4749,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4607,7 +4757,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4615,7 +4765,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4631,7 +4781,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4639,7 +4789,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4647,7 +4797,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -4672,7 +4822,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4693,7 +4843,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4701,7 +4851,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4709,7 +4859,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4717,7 +4867,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4725,7 +4875,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4733,7 +4883,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4741,7 +4891,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4749,7 +4899,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4757,7 +4907,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4765,7 +4915,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4773,7 +4923,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4781,7 +4931,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,7 +4947,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4805,7 +4955,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4813,7 +4963,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4821,7 +4971,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4829,7 +4979,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4837,7 +4987,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4845,7 +4995,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4853,7 +5003,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4861,7 +5011,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4869,7 +5019,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4877,7 +5027,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4885,7 +5035,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4893,7 +5043,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4926,7 +5076,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4947,7 +5097,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4955,7 +5105,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4963,7 +5113,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4971,7 +5121,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4979,7 +5129,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4987,7 +5137,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4995,7 +5145,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5003,7 +5153,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5011,7 +5161,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5019,7 +5169,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5027,7 +5177,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5035,7 +5185,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5043,7 +5193,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5051,7 +5201,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5059,7 +5209,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5067,7 +5217,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5075,7 +5225,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5083,7 +5233,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5091,7 +5241,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5099,7 +5249,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5107,7 +5257,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>